<commit_message>
Agregar fuente de preguntas
</commit_message>
<xml_diff>
--- a/data/quest.xlsx
+++ b/data/quest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Laboratorio Ciencia Social Abierta\encuesta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\kevin\Documents\Laboratorio Ciencia Social Abierta\encuesta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE537BA1-3AC8-43DE-B5BC-B6080E8AA365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA99E1-28DD-4BCF-8896-DC9708AB23F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="312">
   <si>
     <t>varmodule</t>
   </si>
@@ -514,9 +514,6 @@
     <t>data01</t>
   </si>
   <si>
-    <t>¿Qué tan familiarizado está con los principios FAIR (ubicable, accesible, interoperable y reutilizable en español?</t>
-  </si>
-  <si>
     <t>Los/as investigadores no pueden seguir los principios FAIR debido a la falta de capacitación y apoyo adecuados</t>
   </si>
   <si>
@@ -887,6 +884,78 @@
   </si>
   <si>
     <t>info05</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Lopez-cardenas &amp; Cubero-Castillo, 2021; Pardo Martinez &amp; Poveda, 2018</t>
+  </si>
+  <si>
+    <t>Pardo Martinez &amp; Poveda, 2018</t>
+  </si>
+  <si>
+    <t>sturmer, et. Al 2017</t>
+  </si>
+  <si>
+    <t>sturmer, et al 2017; Chin, et al, 2021</t>
+  </si>
+  <si>
+    <t>Chin, et al, 2021</t>
+  </si>
+  <si>
+    <t>sturmer, et al 2017; Chin, et al, 2021; Ljubenkovic, et al, 2021</t>
+  </si>
+  <si>
+    <t>Chin, et al, 2021; Ljubenkovic, et al, 2021</t>
+  </si>
+  <si>
+    <t>¿Qué tan familiarizado está con los principios FAIR (ubicable, accesible, interoperable y reutilizable, en español)?</t>
+  </si>
+  <si>
+    <t>Delikoura &amp; Kouis, 2021</t>
+  </si>
+  <si>
+    <t>Zhu, 2020</t>
+  </si>
+  <si>
+    <t>Hodonu-wusu, et al, 2020</t>
+  </si>
+  <si>
+    <t>Federer et al, 2015</t>
+  </si>
+  <si>
+    <t>Enke et al, 2012</t>
+  </si>
+  <si>
+    <t>Baker, 2016</t>
+  </si>
+  <si>
+    <t>Hail et al, 2020</t>
+  </si>
+  <si>
+    <t>Hail et al, 2020; Baker, 2016</t>
+  </si>
+  <si>
+    <t>Knudtson, et al, 2019</t>
+  </si>
+  <si>
+    <t>Hail et al, 2020; Baker, 2016; Knudtson, et al, 2019</t>
+  </si>
+  <si>
+    <t>Gross &amp; Ryan, 2015</t>
+  </si>
+  <si>
+    <t>Rodriguez, 2014</t>
+  </si>
+  <si>
+    <t>Narayan, et al, 2018</t>
+  </si>
+  <si>
+    <t>Lacey, et al, 2020</t>
+  </si>
+  <si>
+    <t>Rowley, et al, 2017</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,9 +1326,9 @@
     <col min="4" max="4" width="159" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1276,8 +1345,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1293,8 +1365,11 @@
       <c r="F2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1313,8 +1388,11 @@
       <c r="F3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1333,8 +1411,11 @@
       <c r="F4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1353,8 +1434,11 @@
       <c r="F5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1373,8 +1457,11 @@
       <c r="F6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1393,8 +1480,11 @@
       <c r="F7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1413,8 +1503,11 @@
       <c r="F8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1433,8 +1526,11 @@
       <c r="F9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1453,8 +1549,11 @@
       <c r="F10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1473,8 +1572,11 @@
       <c r="F11" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1493,8 +1595,11 @@
       <c r="F12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1513,8 +1618,11 @@
       <c r="F13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1533,8 +1641,11 @@
       <c r="F14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1553,8 +1664,11 @@
       <c r="F15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1573,8 +1687,11 @@
       <c r="F16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1593,8 +1710,11 @@
       <c r="F17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1613,8 +1733,11 @@
       <c r="F18" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1633,8 +1756,11 @@
       <c r="F19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1653,8 +1779,11 @@
       <c r="F20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1673,8 +1802,11 @@
       <c r="F21" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1693,8 +1825,11 @@
       <c r="F22" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1713,8 +1848,11 @@
       <c r="F23" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1733,8 +1871,11 @@
       <c r="F24" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1753,8 +1894,11 @@
       <c r="F25" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1773,8 +1917,11 @@
       <c r="F26" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1793,8 +1940,11 @@
       <c r="F27" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1813,8 +1963,11 @@
       <c r="F28" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1833,8 +1986,11 @@
       <c r="F29" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1853,8 +2009,11 @@
       <c r="F30" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1873,8 +2032,11 @@
       <c r="F31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1893,8 +2055,11 @@
       <c r="F32" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1913,8 +2078,11 @@
       <c r="F33" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1933,8 +2101,11 @@
       <c r="F34" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1953,8 +2124,11 @@
       <c r="F35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1973,8 +2147,11 @@
       <c r="F36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1993,8 +2170,11 @@
       <c r="F37" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2013,8 +2193,11 @@
       <c r="F38" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -2033,8 +2216,11 @@
       <c r="F39" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -2045,13 +2231,16 @@
         <v>163</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>296</v>
       </c>
       <c r="F40" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="G40" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2059,16 +2248,19 @@
         <v>162</v>
       </c>
       <c r="C41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F41" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2076,16 +2268,19 @@
         <v>162</v>
       </c>
       <c r="C42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F42" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -2093,19 +2288,22 @@
         <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F43" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G43" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2113,19 +2311,22 @@
         <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F44" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G44" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -2133,19 +2334,22 @@
         <v>162</v>
       </c>
       <c r="C45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F45" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G45" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2153,19 +2357,22 @@
         <v>162</v>
       </c>
       <c r="C46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F46" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2173,19 +2380,22 @@
         <v>162</v>
       </c>
       <c r="C47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F47" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G47" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2193,19 +2403,22 @@
         <v>162</v>
       </c>
       <c r="C48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G48" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2213,19 +2426,22 @@
         <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G49" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2233,19 +2449,22 @@
         <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F50" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G50" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2253,19 +2472,22 @@
         <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F51" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G51" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2273,19 +2495,22 @@
         <v>162</v>
       </c>
       <c r="C52" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F52" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G52" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2293,19 +2518,22 @@
         <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F53" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G53" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -2313,19 +2541,22 @@
         <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" t="s">
+        <v>193</v>
+      </c>
+      <c r="E54" t="s">
         <v>194</v>
       </c>
-      <c r="E54" t="s">
-        <v>195</v>
-      </c>
       <c r="F54" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G54" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -2333,19 +2564,22 @@
         <v>162</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G55" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -2353,19 +2587,22 @@
         <v>162</v>
       </c>
       <c r="C56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F56" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G56" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2373,19 +2610,22 @@
         <v>162</v>
       </c>
       <c r="C57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F57" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G57" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -2393,636 +2633,726 @@
         <v>162</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F58" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G58" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
       <c r="B59" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" t="s">
         <v>205</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
+        <v>209</v>
+      </c>
+      <c r="F59" t="s">
         <v>206</v>
       </c>
-      <c r="D59" t="s">
-        <v>210</v>
-      </c>
-      <c r="F59" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F60" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G60" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D61" t="s">
+        <v>211</v>
+      </c>
+      <c r="F61" t="s">
         <v>212</v>
       </c>
-      <c r="F61" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C62" t="s">
+        <v>213</v>
+      </c>
+      <c r="D62" t="s">
         <v>214</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
         <v>215</v>
       </c>
-      <c r="F62" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F63" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F64" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C65" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" t="s">
         <v>221</v>
-      </c>
-      <c r="D65" t="s">
-        <v>222</v>
       </c>
       <c r="F65" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C66" t="s">
+        <v>222</v>
+      </c>
+      <c r="D66" t="s">
         <v>223</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>224</v>
       </c>
-      <c r="E66" t="s">
-        <v>225</v>
-      </c>
       <c r="F66" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G66" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F67" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G67" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C68" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F68" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G68" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F69" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G69" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F70" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G70" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F71" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G71" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F72" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G72" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C73" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F73" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G73" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
       <c r="B74" t="s">
+        <v>239</v>
+      </c>
+      <c r="C74" t="s">
         <v>240</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>241</v>
       </c>
-      <c r="D74" t="s">
-        <v>242</v>
-      </c>
       <c r="F74" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="G74" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F75" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C76" t="s">
+        <v>244</v>
+      </c>
+      <c r="D76" t="s">
         <v>245</v>
-      </c>
-      <c r="D76" t="s">
-        <v>246</v>
       </c>
       <c r="F76" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D77" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G77" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D78" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F78" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G78" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F79" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G79" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E80" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F80" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="G80" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C81" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D81" t="s">
+        <v>249</v>
+      </c>
+      <c r="E81" t="s">
         <v>250</v>
       </c>
-      <c r="E81" t="s">
-        <v>251</v>
-      </c>
       <c r="F81" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G81" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C82" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D82" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E82" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F82" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G82" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D83" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F83" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G83" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C84" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D84" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E84" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F84" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G84" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C85" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F85" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G85" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C86" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D86" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F86" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G86" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F87" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G87" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>272</v>
+      </c>
+      <c r="B88" t="s">
+        <v>277</v>
+      </c>
+      <c r="C88" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>273</v>
       </c>
-      <c r="B88" t="s">
-        <v>278</v>
-      </c>
-      <c r="C88" t="s">
-        <v>279</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="B89" t="s">
+        <v>277</v>
+      </c>
+      <c r="C89" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="D89" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>274</v>
       </c>
-      <c r="B89" t="s">
-        <v>278</v>
-      </c>
-      <c r="C89" t="s">
-        <v>281</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="B90" t="s">
+        <v>277</v>
+      </c>
+      <c r="C90" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="D90" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>275</v>
       </c>
-      <c r="B90" t="s">
-        <v>278</v>
-      </c>
-      <c r="C90" t="s">
-        <v>283</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="B91" t="s">
+        <v>277</v>
+      </c>
+      <c r="C91" t="s">
+        <v>286</v>
+      </c>
+      <c r="D91" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>276</v>
       </c>
-      <c r="B91" t="s">
-        <v>278</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="B92" t="s">
+        <v>277</v>
+      </c>
+      <c r="C92" t="s">
         <v>287</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>277</v>
-      </c>
-      <c r="B92" t="s">
-        <v>278</v>
-      </c>
-      <c r="C92" t="s">
-        <v>288</v>
-      </c>
-      <c r="D92" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>